<commit_message>
tweaks to template and model query
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_17_rpt_P_Status_MostRecent.xlsx
+++ b/backend/reports/xlsx/Tab_17_rpt_P_Status_MostRecent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9CD4B9-BC33-2F45-BD32-9043C5EC9AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C45623-76B6-5340-AC3A-6F2790D533F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="520" windowWidth="25600" windowHeight="21100" activeTab="3" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="25600" yWindow="520" windowWidth="25600" windowHeight="21100" activeTab="1" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="76">
   <si>
     <t>Project Manager:</t>
   </si>
@@ -167,9 +167,6 @@
     <t>{#p=d.project}</t>
   </si>
   <si>
-    <t>{#a=d.alignment}</t>
-  </si>
-  <si>
     <t>{#s=d.status}</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>{$p.project_name}</t>
   </si>
   <si>
-    <t>{$a.description}</t>
-  </si>
-  <si>
     <t>{$p.goals}</t>
   </si>
   <si>
@@ -270,6 +264,9 @@
   </si>
   <si>
     <t>Reporting Date: {$prjstat.status_date}</t>
+  </si>
+  <si>
+    <t>{$p.strategic_alignment}</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1778,7 @@
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -1795,7 +1792,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="33"/>
       <c r="E2" s="33"/>
@@ -1813,9 +1810,6 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1">
       <c r="A4" s="5" t="s">
@@ -1828,13 +1822,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -1864,19 +1858,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -1905,13 +1899,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1961,7 +1955,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
@@ -1981,7 +1975,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="64" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C14" s="64"/>
       <c r="D14" s="64"/>
@@ -3613,8 +3607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBFCAC8-5881-134F-AB09-DAB459246A80}">
   <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -3623,12 +3617,12 @@
     <col min="2" max="2" width="25.33203125" style="34" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="34" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="4" style="46" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="34" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" style="46" customWidth="1"/>
     <col min="7" max="7" width="8.5" style="34" customWidth="1"/>
-    <col min="8" max="8" width="4" style="46" customWidth="1"/>
+    <col min="8" max="8" width="3.83203125" style="46" customWidth="1"/>
     <col min="9" max="9" width="11.1640625" style="34" customWidth="1"/>
-    <col min="10" max="10" width="4.5" style="46" customWidth="1"/>
+    <col min="10" max="10" width="3.83203125" style="46" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="34"/>
   </cols>
   <sheetData>
@@ -3641,21 +3635,21 @@
         <v>11</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E1" s="51"/>
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
       <c r="I1" s="49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J1" s="49"/>
       <c r="M1" s="38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="60" customFormat="1" ht="32" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="60" customFormat="1">
       <c r="A2" s="52" t="s">
         <v>15</v>
       </c>
@@ -3666,7 +3660,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="56" t="s">
         <v>17</v>
@@ -4448,7 +4442,7 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1">
@@ -4473,38 +4467,38 @@
       </c>
       <c r="J2" s="28"/>
       <c r="K2" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="22" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="I3" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="J3" s="35" t="s">
         <v>69</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="22" customHeight="1">
       <c r="A4" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -5045,7 +5039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D139B54-76DF-B047-B773-CF046491ECCD}">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -5079,32 +5073,32 @@
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" customHeight="1">
       <c r="A3" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
       <c r="E3" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6">

</xml_diff>

<commit_message>
fix tab 17 strategic alignment carbone templating string
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_17_rpt_P_Status_MostRecent.xlsx
+++ b/backend/reports/xlsx/Tab_17_rpt_P_Status_MostRecent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A2ABDF-40F1-C942-9F8C-19A6BAB28A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0599183-0D21-A240-9527-FA99E1904589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="520" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Info" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>{$p.project_name}</t>
   </si>
   <si>
-    <t>{$a.description}</t>
-  </si>
-  <si>
     <t>{$p.goals}</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>Reporting Date: {$prjstat.status_date}</t>
+  </si>
+  <si>
+    <t>{$p.strategic_alignment}</t>
   </si>
 </sst>
 </file>
@@ -274,7 +274,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -503,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -527,24 +527,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -562,43 +544,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
@@ -608,15 +575,11 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -631,10 +594,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,7 +606,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -655,372 +618,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FFFFFF00"/>
@@ -1775,14 +1408,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="31" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16" t="s">
+      <c r="A1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
       <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
         <v>41</v>
@@ -1791,24 +1424,24 @@
     <row r="2" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1">
@@ -1822,7 +1455,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>2</v>
@@ -1904,11 +1537,11 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="11" t="s">
@@ -1934,53 +1567,53 @@
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="11"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
+      <c r="B12" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="11"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:8" ht="40">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="11" t="s">
@@ -3613,764 +3246,764 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="34" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="34" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="34" customWidth="1"/>
-    <col min="6" max="6" width="3.83203125" style="46" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="34" customWidth="1"/>
-    <col min="8" max="8" width="3.83203125" style="46" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="34" customWidth="1"/>
-    <col min="10" max="10" width="3.83203125" style="46" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="34"/>
+    <col min="1" max="1" width="11.1640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="25" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" style="33" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="25" customWidth="1"/>
+    <col min="8" max="8" width="3.83203125" style="33" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="3.83203125" style="33" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="38" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:13" ht="21" customHeight="1">
+      <c r="A1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="49" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="54"/>
+      <c r="M1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="49"/>
-      <c r="M1" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="60" customFormat="1">
-      <c r="A2" s="52" t="s">
+    </row>
+    <row r="2" spans="1:13" s="45" customFormat="1">
+      <c r="A2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="56" t="s">
+      <c r="D2" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="59"/>
-    </row>
-    <row r="3" spans="1:13" s="43" customFormat="1" ht="21" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="K2" s="44"/>
+    </row>
+    <row r="3" spans="1:13" s="31" customFormat="1" ht="21" customHeight="1">
+      <c r="A3" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
-    </row>
-    <row r="4" spans="1:13" s="39" customFormat="1" ht="21" customHeight="1">
-      <c r="A4" s="44" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="30"/>
+    </row>
+    <row r="4" spans="1:13" s="28" customFormat="1" ht="21" customHeight="1">
+      <c r="A4" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="40"/>
-    </row>
-    <row r="5" spans="1:13" s="43" customFormat="1" ht="21" customHeight="1">
-      <c r="A5" s="41" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="29"/>
+    </row>
+    <row r="5" spans="1:13" s="31" customFormat="1" ht="21" customHeight="1">
+      <c r="A5" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="42"/>
-    </row>
-    <row r="6" spans="1:13" s="39" customFormat="1" ht="21" customHeight="1">
-      <c r="A6" s="44" t="s">
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="30"/>
+    </row>
+    <row r="6" spans="1:13" s="28" customFormat="1" ht="21" customHeight="1">
+      <c r="A6" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="40"/>
-    </row>
-    <row r="7" spans="1:13" s="43" customFormat="1" ht="21" customHeight="1">
-      <c r="A7" s="41" t="s">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="1:13" s="31" customFormat="1" ht="21" customHeight="1">
+      <c r="A7" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="42"/>
-    </row>
-    <row r="8" spans="1:13" s="39" customFormat="1" ht="21" customHeight="1">
-      <c r="A8" s="44" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="30"/>
+    </row>
+    <row r="8" spans="1:13" s="28" customFormat="1" ht="21" customHeight="1">
+      <c r="A8" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="40"/>
-    </row>
-    <row r="9" spans="1:13" s="43" customFormat="1" ht="21" customHeight="1">
-      <c r="A9" s="41" t="s">
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="1:13" s="31" customFormat="1" ht="21" customHeight="1">
+      <c r="A9" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="42"/>
-    </row>
-    <row r="10" spans="1:13" s="39" customFormat="1" ht="21" customHeight="1">
-      <c r="A10" s="44" t="s">
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:13" s="28" customFormat="1" ht="21" customHeight="1">
+      <c r="A10" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="40"/>
-    </row>
-    <row r="11" spans="1:13" s="39" customFormat="1" ht="21" customHeight="1">
-      <c r="F11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="J11" s="40"/>
-    </row>
-    <row r="12" spans="1:13" s="39" customFormat="1">
-      <c r="F12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="J12" s="40"/>
-    </row>
-    <row r="13" spans="1:13" s="39" customFormat="1">
-      <c r="F13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="J13" s="40"/>
-    </row>
-    <row r="14" spans="1:13" s="39" customFormat="1">
-      <c r="F14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="J14" s="40"/>
-    </row>
-    <row r="15" spans="1:13" s="39" customFormat="1">
-      <c r="F15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="J15" s="40"/>
-    </row>
-    <row r="16" spans="1:13" s="39" customFormat="1">
-      <c r="F16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="J16" s="40"/>
-    </row>
-    <row r="17" spans="6:10" s="39" customFormat="1">
-      <c r="F17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="J17" s="40"/>
-    </row>
-    <row r="18" spans="6:10" s="39" customFormat="1">
-      <c r="F18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="J18" s="40"/>
-    </row>
-    <row r="19" spans="6:10" s="39" customFormat="1">
-      <c r="F19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="J19" s="40"/>
-    </row>
-    <row r="20" spans="6:10" s="39" customFormat="1">
-      <c r="F20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="J20" s="40"/>
-    </row>
-    <row r="21" spans="6:10" s="39" customFormat="1">
-      <c r="F21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="J21" s="40"/>
-    </row>
-    <row r="22" spans="6:10" s="39" customFormat="1">
-      <c r="F22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="J22" s="40"/>
-    </row>
-    <row r="23" spans="6:10" s="39" customFormat="1">
-      <c r="F23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="J23" s="40"/>
-    </row>
-    <row r="24" spans="6:10" s="39" customFormat="1">
-      <c r="F24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="J24" s="40"/>
-    </row>
-    <row r="25" spans="6:10" s="39" customFormat="1">
-      <c r="F25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="J25" s="40"/>
-    </row>
-    <row r="26" spans="6:10" s="39" customFormat="1">
-      <c r="F26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="J26" s="40"/>
-    </row>
-    <row r="27" spans="6:10" s="39" customFormat="1">
-      <c r="F27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="J27" s="40"/>
-    </row>
-    <row r="28" spans="6:10" s="39" customFormat="1">
-      <c r="F28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="J28" s="40"/>
-    </row>
-    <row r="29" spans="6:10" s="39" customFormat="1">
-      <c r="F29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="J29" s="40"/>
-    </row>
-    <row r="30" spans="6:10" s="39" customFormat="1">
-      <c r="F30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="J30" s="40"/>
-    </row>
-    <row r="31" spans="6:10" s="39" customFormat="1">
-      <c r="F31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="J31" s="40"/>
-    </row>
-    <row r="32" spans="6:10" s="39" customFormat="1">
-      <c r="F32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="J32" s="40"/>
-    </row>
-    <row r="33" spans="6:10" s="39" customFormat="1">
-      <c r="F33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="J33" s="40"/>
-    </row>
-    <row r="34" spans="6:10" s="39" customFormat="1">
-      <c r="F34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="J34" s="40"/>
-    </row>
-    <row r="35" spans="6:10" s="39" customFormat="1">
-      <c r="F35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="J35" s="40"/>
-    </row>
-    <row r="36" spans="6:10" s="39" customFormat="1">
-      <c r="F36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="J36" s="40"/>
-    </row>
-    <row r="37" spans="6:10" s="39" customFormat="1">
-      <c r="F37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="J37" s="40"/>
-    </row>
-    <row r="38" spans="6:10" s="39" customFormat="1">
-      <c r="F38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="J38" s="40"/>
-    </row>
-    <row r="39" spans="6:10" s="39" customFormat="1">
-      <c r="F39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="J39" s="40"/>
-    </row>
-    <row r="40" spans="6:10" s="39" customFormat="1">
-      <c r="F40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="J40" s="40"/>
-    </row>
-    <row r="41" spans="6:10" s="39" customFormat="1">
-      <c r="F41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="J41" s="40"/>
-    </row>
-    <row r="42" spans="6:10" s="39" customFormat="1">
-      <c r="F42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="J42" s="40"/>
-    </row>
-    <row r="43" spans="6:10" s="39" customFormat="1">
-      <c r="F43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="J43" s="40"/>
-    </row>
-    <row r="44" spans="6:10" s="39" customFormat="1">
-      <c r="F44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="J44" s="40"/>
-    </row>
-    <row r="45" spans="6:10" s="39" customFormat="1">
-      <c r="F45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="J45" s="40"/>
-    </row>
-    <row r="46" spans="6:10" s="39" customFormat="1">
-      <c r="F46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="J46" s="40"/>
-    </row>
-    <row r="47" spans="6:10" s="39" customFormat="1">
-      <c r="F47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="J47" s="40"/>
-    </row>
-    <row r="48" spans="6:10" s="39" customFormat="1">
-      <c r="F48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="J48" s="40"/>
-    </row>
-    <row r="49" spans="6:10" s="39" customFormat="1">
-      <c r="F49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="J49" s="40"/>
-    </row>
-    <row r="50" spans="6:10" s="39" customFormat="1">
-      <c r="F50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="J50" s="40"/>
-    </row>
-    <row r="51" spans="6:10" s="39" customFormat="1">
-      <c r="F51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="J51" s="40"/>
-    </row>
-    <row r="52" spans="6:10" s="39" customFormat="1">
-      <c r="F52" s="45"/>
-      <c r="H52" s="45"/>
-      <c r="J52" s="40"/>
-    </row>
-    <row r="53" spans="6:10" s="39" customFormat="1">
-      <c r="F53" s="45"/>
-      <c r="H53" s="45"/>
-      <c r="J53" s="40"/>
-    </row>
-    <row r="54" spans="6:10" s="39" customFormat="1">
-      <c r="F54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="J54" s="40"/>
-    </row>
-    <row r="55" spans="6:10" s="39" customFormat="1">
-      <c r="F55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="J55" s="40"/>
-    </row>
-    <row r="56" spans="6:10" s="39" customFormat="1">
-      <c r="F56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="J56" s="40"/>
-    </row>
-    <row r="57" spans="6:10" s="39" customFormat="1">
-      <c r="F57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="J57" s="40"/>
-    </row>
-    <row r="58" spans="6:10" s="39" customFormat="1">
-      <c r="F58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="J58" s="40"/>
-    </row>
-    <row r="59" spans="6:10" s="39" customFormat="1">
-      <c r="F59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="J59" s="40"/>
-    </row>
-    <row r="60" spans="6:10" s="39" customFormat="1">
-      <c r="F60" s="45"/>
-      <c r="H60" s="45"/>
-      <c r="J60" s="40"/>
-    </row>
-    <row r="61" spans="6:10" s="39" customFormat="1">
-      <c r="F61" s="45"/>
-      <c r="H61" s="45"/>
-      <c r="J61" s="40"/>
-    </row>
-    <row r="62" spans="6:10" s="39" customFormat="1">
-      <c r="F62" s="45"/>
-      <c r="H62" s="45"/>
-      <c r="J62" s="40"/>
-    </row>
-    <row r="63" spans="6:10" s="39" customFormat="1">
-      <c r="F63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="J63" s="40"/>
-    </row>
-    <row r="64" spans="6:10" s="39" customFormat="1">
-      <c r="F64" s="45"/>
-      <c r="H64" s="45"/>
-      <c r="J64" s="40"/>
-    </row>
-    <row r="65" spans="6:10" s="39" customFormat="1">
-      <c r="F65" s="45"/>
-      <c r="H65" s="45"/>
-      <c r="J65" s="40"/>
-    </row>
-    <row r="66" spans="6:10" s="39" customFormat="1">
-      <c r="F66" s="45"/>
-      <c r="H66" s="45"/>
-      <c r="J66" s="40"/>
-    </row>
-    <row r="67" spans="6:10" s="39" customFormat="1">
-      <c r="F67" s="45"/>
-      <c r="H67" s="45"/>
-      <c r="J67" s="40"/>
-    </row>
-    <row r="68" spans="6:10" s="39" customFormat="1">
-      <c r="F68" s="45"/>
-      <c r="H68" s="45"/>
-      <c r="J68" s="40"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:13" s="28" customFormat="1" ht="21" customHeight="1">
+      <c r="F11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:13" s="28" customFormat="1">
+      <c r="F12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:13" s="28" customFormat="1">
+      <c r="F13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="J13" s="29"/>
+    </row>
+    <row r="14" spans="1:13" s="28" customFormat="1">
+      <c r="F14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="J14" s="29"/>
+    </row>
+    <row r="15" spans="1:13" s="28" customFormat="1">
+      <c r="F15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="J15" s="29"/>
+    </row>
+    <row r="16" spans="1:13" s="28" customFormat="1">
+      <c r="F16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="6:10" s="28" customFormat="1">
+      <c r="F17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="J17" s="29"/>
+    </row>
+    <row r="18" spans="6:10" s="28" customFormat="1">
+      <c r="F18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="J18" s="29"/>
+    </row>
+    <row r="19" spans="6:10" s="28" customFormat="1">
+      <c r="F19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="J19" s="29"/>
+    </row>
+    <row r="20" spans="6:10" s="28" customFormat="1">
+      <c r="F20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="6:10" s="28" customFormat="1">
+      <c r="F21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="6:10" s="28" customFormat="1">
+      <c r="F22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="6:10" s="28" customFormat="1">
+      <c r="F23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="6:10" s="28" customFormat="1">
+      <c r="F24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="J24" s="29"/>
+    </row>
+    <row r="25" spans="6:10" s="28" customFormat="1">
+      <c r="F25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="J25" s="29"/>
+    </row>
+    <row r="26" spans="6:10" s="28" customFormat="1">
+      <c r="F26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="6:10" s="28" customFormat="1">
+      <c r="F27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="6:10" s="28" customFormat="1">
+      <c r="F28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="J28" s="29"/>
+    </row>
+    <row r="29" spans="6:10" s="28" customFormat="1">
+      <c r="F29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="6:10" s="28" customFormat="1">
+      <c r="F30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="6:10" s="28" customFormat="1">
+      <c r="F31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="J31" s="29"/>
+    </row>
+    <row r="32" spans="6:10" s="28" customFormat="1">
+      <c r="F32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="6:10" s="28" customFormat="1">
+      <c r="F33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="J33" s="29"/>
+    </row>
+    <row r="34" spans="6:10" s="28" customFormat="1">
+      <c r="F34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="6:10" s="28" customFormat="1">
+      <c r="F35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="J35" s="29"/>
+    </row>
+    <row r="36" spans="6:10" s="28" customFormat="1">
+      <c r="F36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="J36" s="29"/>
+    </row>
+    <row r="37" spans="6:10" s="28" customFormat="1">
+      <c r="F37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="J37" s="29"/>
+    </row>
+    <row r="38" spans="6:10" s="28" customFormat="1">
+      <c r="F38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="J38" s="29"/>
+    </row>
+    <row r="39" spans="6:10" s="28" customFormat="1">
+      <c r="F39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="J39" s="29"/>
+    </row>
+    <row r="40" spans="6:10" s="28" customFormat="1">
+      <c r="F40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="J40" s="29"/>
+    </row>
+    <row r="41" spans="6:10" s="28" customFormat="1">
+      <c r="F41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="J41" s="29"/>
+    </row>
+    <row r="42" spans="6:10" s="28" customFormat="1">
+      <c r="F42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="J42" s="29"/>
+    </row>
+    <row r="43" spans="6:10" s="28" customFormat="1">
+      <c r="F43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="J43" s="29"/>
+    </row>
+    <row r="44" spans="6:10" s="28" customFormat="1">
+      <c r="F44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="J44" s="29"/>
+    </row>
+    <row r="45" spans="6:10" s="28" customFormat="1">
+      <c r="F45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="J45" s="29"/>
+    </row>
+    <row r="46" spans="6:10" s="28" customFormat="1">
+      <c r="F46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="J46" s="29"/>
+    </row>
+    <row r="47" spans="6:10" s="28" customFormat="1">
+      <c r="F47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="J47" s="29"/>
+    </row>
+    <row r="48" spans="6:10" s="28" customFormat="1">
+      <c r="F48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="J48" s="29"/>
+    </row>
+    <row r="49" spans="6:10" s="28" customFormat="1">
+      <c r="F49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="J49" s="29"/>
+    </row>
+    <row r="50" spans="6:10" s="28" customFormat="1">
+      <c r="F50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="J50" s="29"/>
+    </row>
+    <row r="51" spans="6:10" s="28" customFormat="1">
+      <c r="F51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="J51" s="29"/>
+    </row>
+    <row r="52" spans="6:10" s="28" customFormat="1">
+      <c r="F52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="J52" s="29"/>
+    </row>
+    <row r="53" spans="6:10" s="28" customFormat="1">
+      <c r="F53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="J53" s="29"/>
+    </row>
+    <row r="54" spans="6:10" s="28" customFormat="1">
+      <c r="F54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="J54" s="29"/>
+    </row>
+    <row r="55" spans="6:10" s="28" customFormat="1">
+      <c r="F55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="J55" s="29"/>
+    </row>
+    <row r="56" spans="6:10" s="28" customFormat="1">
+      <c r="F56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="J56" s="29"/>
+    </row>
+    <row r="57" spans="6:10" s="28" customFormat="1">
+      <c r="F57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="J57" s="29"/>
+    </row>
+    <row r="58" spans="6:10" s="28" customFormat="1">
+      <c r="F58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="J58" s="29"/>
+    </row>
+    <row r="59" spans="6:10" s="28" customFormat="1">
+      <c r="F59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="J59" s="29"/>
+    </row>
+    <row r="60" spans="6:10" s="28" customFormat="1">
+      <c r="F60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="J60" s="29"/>
+    </row>
+    <row r="61" spans="6:10" s="28" customFormat="1">
+      <c r="F61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="J61" s="29"/>
+    </row>
+    <row r="62" spans="6:10" s="28" customFormat="1">
+      <c r="F62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="J62" s="29"/>
+    </row>
+    <row r="63" spans="6:10" s="28" customFormat="1">
+      <c r="F63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="J63" s="29"/>
+    </row>
+    <row r="64" spans="6:10" s="28" customFormat="1">
+      <c r="F64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="J64" s="29"/>
+    </row>
+    <row r="65" spans="6:10" s="28" customFormat="1">
+      <c r="F65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="J65" s="29"/>
+    </row>
+    <row r="66" spans="6:10" s="28" customFormat="1">
+      <c r="F66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="J66" s="29"/>
+    </row>
+    <row r="67" spans="6:10" s="28" customFormat="1">
+      <c r="F67" s="32"/>
+      <c r="H67" s="32"/>
+      <c r="J67" s="29"/>
+    </row>
+    <row r="68" spans="6:10" s="28" customFormat="1">
+      <c r="F68" s="32"/>
+      <c r="H68" s="32"/>
+      <c r="J68" s="29"/>
     </row>
     <row r="69" spans="6:10">
-      <c r="J69" s="47"/>
+      <c r="J69" s="34"/>
     </row>
     <row r="70" spans="6:10">
-      <c r="J70" s="47"/>
+      <c r="J70" s="34"/>
     </row>
     <row r="71" spans="6:10">
-      <c r="J71" s="47"/>
+      <c r="J71" s="34"/>
     </row>
     <row r="72" spans="6:10">
-      <c r="J72" s="47"/>
+      <c r="J72" s="34"/>
     </row>
     <row r="73" spans="6:10">
-      <c r="J73" s="47"/>
+      <c r="J73" s="34"/>
     </row>
     <row r="74" spans="6:10">
-      <c r="J74" s="47"/>
+      <c r="J74" s="34"/>
     </row>
     <row r="75" spans="6:10">
-      <c r="J75" s="47"/>
+      <c r="J75" s="34"/>
     </row>
     <row r="76" spans="6:10">
-      <c r="J76" s="47"/>
+      <c r="J76" s="34"/>
     </row>
     <row r="77" spans="6:10">
-      <c r="J77" s="47"/>
+      <c r="J77" s="34"/>
     </row>
     <row r="78" spans="6:10">
-      <c r="J78" s="47"/>
+      <c r="J78" s="34"/>
     </row>
     <row r="79" spans="6:10">
-      <c r="J79" s="47"/>
+      <c r="J79" s="34"/>
     </row>
     <row r="80" spans="6:10">
-      <c r="J80" s="47"/>
+      <c r="J80" s="34"/>
     </row>
     <row r="81" spans="10:10">
-      <c r="J81" s="47"/>
+      <c r="J81" s="34"/>
     </row>
     <row r="82" spans="10:10">
-      <c r="J82" s="47"/>
+      <c r="J82" s="34"/>
     </row>
     <row r="83" spans="10:10">
-      <c r="J83" s="47"/>
+      <c r="J83" s="34"/>
     </row>
     <row r="84" spans="10:10">
-      <c r="J84" s="47"/>
+      <c r="J84" s="34"/>
     </row>
     <row r="85" spans="10:10">
-      <c r="J85" s="47"/>
+      <c r="J85" s="34"/>
     </row>
     <row r="86" spans="10:10">
-      <c r="J86" s="47"/>
+      <c r="J86" s="34"/>
     </row>
     <row r="87" spans="10:10">
-      <c r="J87" s="47"/>
+      <c r="J87" s="34"/>
     </row>
     <row r="88" spans="10:10">
-      <c r="J88" s="47"/>
+      <c r="J88" s="34"/>
     </row>
     <row r="89" spans="10:10">
-      <c r="J89" s="47"/>
+      <c r="J89" s="34"/>
     </row>
     <row r="90" spans="10:10">
-      <c r="J90" s="47"/>
+      <c r="J90" s="34"/>
     </row>
     <row r="91" spans="10:10">
-      <c r="J91" s="47"/>
+      <c r="J91" s="34"/>
     </row>
     <row r="92" spans="10:10">
-      <c r="J92" s="47"/>
+      <c r="J92" s="34"/>
     </row>
     <row r="93" spans="10:10">
-      <c r="J93" s="47"/>
+      <c r="J93" s="34"/>
     </row>
     <row r="94" spans="10:10">
-      <c r="J94" s="47"/>
+      <c r="J94" s="34"/>
     </row>
     <row r="95" spans="10:10">
-      <c r="J95" s="47"/>
+      <c r="J95" s="34"/>
     </row>
     <row r="96" spans="10:10">
-      <c r="J96" s="47"/>
+      <c r="J96" s="34"/>
     </row>
     <row r="97" spans="10:10">
-      <c r="J97" s="47"/>
+      <c r="J97" s="34"/>
     </row>
     <row r="98" spans="10:10">
-      <c r="J98" s="47"/>
+      <c r="J98" s="34"/>
     </row>
     <row r="99" spans="10:10">
-      <c r="J99" s="47"/>
+      <c r="J99" s="34"/>
     </row>
     <row r="100" spans="10:10">
-      <c r="J100" s="47"/>
+      <c r="J100" s="34"/>
     </row>
     <row r="101" spans="10:10">
-      <c r="J101" s="47"/>
+      <c r="J101" s="34"/>
     </row>
     <row r="102" spans="10:10">
-      <c r="J102" s="47"/>
+      <c r="J102" s="34"/>
     </row>
     <row r="103" spans="10:10">
-      <c r="J103" s="47"/>
+      <c r="J103" s="34"/>
     </row>
     <row r="104" spans="10:10">
-      <c r="J104" s="47"/>
+      <c r="J104" s="34"/>
     </row>
     <row r="105" spans="10:10">
-      <c r="J105" s="47"/>
+      <c r="J105" s="34"/>
     </row>
     <row r="106" spans="10:10">
-      <c r="J106" s="47"/>
+      <c r="J106" s="34"/>
     </row>
     <row r="107" spans="10:10">
-      <c r="J107" s="47"/>
+      <c r="J107" s="34"/>
     </row>
     <row r="108" spans="10:10">
-      <c r="J108" s="47"/>
+      <c r="J108" s="34"/>
     </row>
     <row r="109" spans="10:10">
-      <c r="J109" s="47"/>
+      <c r="J109" s="34"/>
     </row>
     <row r="110" spans="10:10">
-      <c r="J110" s="47"/>
+      <c r="J110" s="34"/>
     </row>
     <row r="111" spans="10:10">
-      <c r="J111" s="47"/>
+      <c r="J111" s="34"/>
     </row>
     <row r="112" spans="10:10">
-      <c r="J112" s="47"/>
+      <c r="J112" s="34"/>
     </row>
     <row r="113" spans="10:10">
-      <c r="J113" s="47"/>
+      <c r="J113" s="34"/>
     </row>
     <row r="114" spans="10:10">
-      <c r="J114" s="47"/>
+      <c r="J114" s="34"/>
     </row>
     <row r="115" spans="10:10">
-      <c r="J115" s="47"/>
+      <c r="J115" s="34"/>
     </row>
     <row r="116" spans="10:10">
-      <c r="J116" s="47"/>
+      <c r="J116" s="34"/>
     </row>
     <row r="117" spans="10:10">
-      <c r="J117" s="47"/>
+      <c r="J117" s="34"/>
     </row>
     <row r="118" spans="10:10">
-      <c r="J118" s="47"/>
+      <c r="J118" s="34"/>
     </row>
     <row r="119" spans="10:10">
-      <c r="J119" s="47"/>
+      <c r="J119" s="34"/>
     </row>
     <row r="120" spans="10:10">
-      <c r="J120" s="47"/>
+      <c r="J120" s="34"/>
     </row>
     <row r="121" spans="10:10">
-      <c r="J121" s="47"/>
+      <c r="J121" s="34"/>
     </row>
     <row r="122" spans="10:10">
-      <c r="J122" s="47"/>
+      <c r="J122" s="34"/>
     </row>
     <row r="123" spans="10:10">
-      <c r="J123" s="47"/>
+      <c r="J123" s="34"/>
     </row>
     <row r="124" spans="10:10">
-      <c r="J124" s="47"/>
+      <c r="J124" s="34"/>
     </row>
     <row r="125" spans="10:10">
-      <c r="J125" s="47"/>
+      <c r="J125" s="34"/>
     </row>
     <row r="126" spans="10:10">
-      <c r="J126" s="47"/>
+      <c r="J126" s="34"/>
     </row>
     <row r="127" spans="10:10">
-      <c r="J127" s="47"/>
+      <c r="J127" s="34"/>
     </row>
     <row r="128" spans="10:10">
-      <c r="J128" s="47"/>
+      <c r="J128" s="34"/>
     </row>
     <row r="129" spans="10:10">
-      <c r="J129" s="47"/>
+      <c r="J129" s="34"/>
     </row>
     <row r="130" spans="10:10">
-      <c r="J130" s="47"/>
+      <c r="J130" s="34"/>
     </row>
     <row r="131" spans="10:10">
-      <c r="J131" s="47"/>
+      <c r="J131" s="34"/>
     </row>
     <row r="132" spans="10:10">
-      <c r="J132" s="47"/>
+      <c r="J132" s="34"/>
     </row>
     <row r="133" spans="10:10">
-      <c r="J133" s="47"/>
+      <c r="J133" s="34"/>
     </row>
     <row r="134" spans="10:10">
-      <c r="J134" s="47"/>
+      <c r="J134" s="34"/>
     </row>
     <row r="135" spans="10:10">
-      <c r="J135" s="47"/>
+      <c r="J135" s="34"/>
     </row>
     <row r="136" spans="10:10">
-      <c r="J136" s="47"/>
+      <c r="J136" s="34"/>
     </row>
     <row r="137" spans="10:10">
-      <c r="J137" s="47"/>
+      <c r="J137" s="34"/>
     </row>
     <row r="138" spans="10:10">
-      <c r="J138" s="47"/>
+      <c r="J138" s="34"/>
     </row>
     <row r="139" spans="10:10">
-      <c r="J139" s="47"/>
+      <c r="J139" s="34"/>
     </row>
     <row r="140" spans="10:10">
-      <c r="J140" s="47"/>
+      <c r="J140" s="34"/>
     </row>
     <row r="141" spans="10:10">
-      <c r="J141" s="47"/>
+      <c r="J141" s="34"/>
     </row>
     <row r="142" spans="10:10">
-      <c r="J142" s="47"/>
+      <c r="J142" s="34"/>
     </row>
     <row r="143" spans="10:10">
-      <c r="J143" s="47"/>
+      <c r="J143" s="34"/>
     </row>
     <row r="144" spans="10:10">
-      <c r="J144" s="47"/>
+      <c r="J144" s="34"/>
     </row>
     <row r="145" spans="10:10">
-      <c r="J145" s="47"/>
+      <c r="J145" s="34"/>
     </row>
     <row r="146" spans="10:10">
-      <c r="J146" s="47"/>
+      <c r="J146" s="34"/>
     </row>
     <row r="147" spans="10:10">
-      <c r="J147" s="47"/>
+      <c r="J147" s="34"/>
     </row>
     <row r="148" spans="10:10">
-      <c r="J148" s="47"/>
+      <c r="J148" s="34"/>
     </row>
     <row r="149" spans="10:10">
-      <c r="J149" s="47"/>
+      <c r="J149" s="34"/>
     </row>
     <row r="150" spans="10:10">
-      <c r="J150" s="47"/>
+      <c r="J150" s="34"/>
     </row>
     <row r="151" spans="10:10">
-      <c r="J151" s="47"/>
+      <c r="J151" s="34"/>
     </row>
     <row r="152" spans="10:10">
-      <c r="J152" s="47"/>
+      <c r="J152" s="34"/>
     </row>
     <row r="153" spans="10:10">
-      <c r="J153" s="47"/>
+      <c r="J153" s="34"/>
     </row>
     <row r="154" spans="10:10">
-      <c r="J154" s="47"/>
+      <c r="J154" s="34"/>
     </row>
     <row r="155" spans="10:10">
-      <c r="J155" s="47"/>
+      <c r="J155" s="34"/>
     </row>
     <row r="156" spans="10:10">
-      <c r="J156" s="47"/>
+      <c r="J156" s="34"/>
     </row>
     <row r="157" spans="10:10">
-      <c r="J157" s="47"/>
+      <c r="J157" s="34"/>
     </row>
     <row r="158" spans="10:10">
-      <c r="J158" s="47"/>
+      <c r="J158" s="34"/>
     </row>
     <row r="159" spans="10:10">
-      <c r="J159" s="47"/>
+      <c r="J159" s="34"/>
     </row>
     <row r="160" spans="10:10">
-      <c r="J160" s="47"/>
+      <c r="J160" s="34"/>
     </row>
     <row r="161" spans="10:10">
-      <c r="J161" s="47"/>
+      <c r="J161" s="34"/>
     </row>
     <row r="162" spans="10:10">
-      <c r="J162" s="47"/>
+      <c r="J162" s="34"/>
     </row>
     <row r="163" spans="10:10">
-      <c r="J163" s="47"/>
+      <c r="J163" s="34"/>
     </row>
     <row r="164" spans="10:10">
-      <c r="J164" s="47"/>
+      <c r="J164" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4384,7 +4017,7 @@
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A6:I6"/>
   </mergeCells>
-  <conditionalFormatting sqref="A11 J11:XFD11 I1 K1:XFD1 A1:E1 A12:XFD1048576 A2:XFD10">
+  <conditionalFormatting sqref="A1:E1 I1 K1:XFD1 A2:XFD10 A11 J11:XFD11 A12:XFD1048576">
     <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
       <formula>AND(ISNUMBER(FIND(",",A1)),VALUE(LEFT(A1,FIND(",",A1)-1))=255,VALUE(MID(A1,FIND(",",A1)+1,FIND(",",A1, FIND(",",A1)+1)-FIND(",",A1)-1))=255,VALUE(MID(A1,FIND(",",A1, FIND(",",A1)+1)+1,LEN(A1)-FIND(",",A1, FIND(",",A1)+1)))=255)</formula>
     </cfRule>
@@ -4421,28 +4054,28 @@
     <col min="4" max="4" width="23.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="4" customWidth="1"/>
     <col min="6" max="6" width="13" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="32"/>
+    <col min="7" max="7" width="13.33203125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="24"/>
     <col min="9" max="9" width="10.83203125" style="4"/>
-    <col min="10" max="10" width="4.83203125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="4.83203125" style="4" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
       <c r="K1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="22" customHeight="1">
@@ -4459,547 +4092,485 @@
       <c r="G2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="22" t="s">
         <v>40</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="28"/>
+      <c r="J2" s="13"/>
       <c r="K2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="22" customHeight="1">
+      <c r="A3" s="58" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="22" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="22" customHeight="1">
+      <c r="A4" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="22" customHeight="1">
-      <c r="A4" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
     </row>
     <row r="5" spans="1:11" ht="22" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
     </row>
     <row r="6" spans="1:11" ht="22" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
     </row>
     <row r="7" spans="1:11" ht="22" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:11" ht="22" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:11" ht="22" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
     </row>
     <row r="10" spans="1:11" ht="22" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
     </row>
     <row r="11" spans="1:11" ht="22" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
     </row>
     <row r="12" spans="1:11" ht="22" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
     </row>
     <row r="13" spans="1:11" ht="22" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
     </row>
     <row r="14" spans="1:11" ht="22" customHeight="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
     </row>
     <row r="15" spans="1:11" ht="22" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
     </row>
     <row r="16" spans="1:11" ht="22" customHeight="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
     </row>
     <row r="17" spans="1:4" ht="22" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
     </row>
     <row r="18" spans="1:4" ht="22" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
     </row>
     <row r="19" spans="1:4" ht="22" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="57"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="57"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="A37" s="57"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="A38" s="57"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="A39" s="57"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="57"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="A41" s="57"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
+      <c r="A42" s="57"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
+      <c r="A43" s="57"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="A44" s="57"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="A45" s="57"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="A47" s="57"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
+      <c r="A48" s="57"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
+      <c r="A49" s="57"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="A50" s="57"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
+      <c r="A51" s="57"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="A53" s="57"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
+      <c r="A54" s="57"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
+      <c r="A55" s="57"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="57"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
+      <c r="A57" s="57"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="18"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
+      <c r="A58" s="57"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
+      <c r="A59" s="57"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
+      <c r="A60" s="57"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
+      <c r="A61" s="57"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
+      <c r="A62" s="57"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
+      <c r="A63" s="57"/>
+      <c r="B63" s="57"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
+      <c r="A64" s="57"/>
+      <c r="B64" s="57"/>
+      <c r="C64" s="57"/>
+      <c r="D64" s="57"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="18"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
+      <c r="A65" s="57"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
+      <c r="A66" s="57"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
+      <c r="A67" s="57"/>
+      <c r="B67" s="57"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
+      <c r="A68" s="57"/>
+      <c r="B68" s="57"/>
+      <c r="C68" s="57"/>
+      <c r="D68" s="57"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
+      <c r="A69" s="57"/>
+      <c r="B69" s="57"/>
+      <c r="C69" s="57"/>
+      <c r="D69" s="57"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
+      <c r="A70" s="57"/>
+      <c r="B70" s="57"/>
+      <c r="C70" s="57"/>
+      <c r="D70" s="57"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
+      <c r="A71" s="57"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="57"/>
+      <c r="D71" s="57"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
+      <c r="A72" s="57"/>
+      <c r="B72" s="57"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="57"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="18"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
+      <c r="A73" s="57"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="57"/>
+      <c r="D73" s="57"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="18"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
+      <c r="A74" s="57"/>
+      <c r="B74" s="57"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="18"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
+      <c r="A75" s="57"/>
+      <c r="B75" s="57"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="18"/>
+      <c r="A76" s="57"/>
+      <c r="B76" s="57"/>
+      <c r="C76" s="57"/>
+      <c r="D76" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
@@ -5013,6 +4584,68 @@
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A75:D75"/>
   </mergeCells>
   <conditionalFormatting sqref="J3:J1048576">
     <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
@@ -5047,302 +4680,302 @@
   <cols>
     <col min="1" max="1" width="49.5" customWidth="1"/>
     <col min="2" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6" style="36" customWidth="1"/>
+    <col min="5" max="5" width="6" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19" customHeight="1">
+      <c r="A3" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19" customHeight="1">
-      <c r="A3" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="27" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="27"/>
+      <c r="A5" s="21"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="27"/>
+      <c r="A6" s="21"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="27"/>
+      <c r="A7" s="21"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="27"/>
+      <c r="A8" s="21"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="27"/>
+      <c r="A9" s="21"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="27"/>
+      <c r="A10" s="21"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="27"/>
+      <c r="A11" s="21"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="27"/>
+      <c r="A12" s="21"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="27"/>
+      <c r="A13" s="21"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="27"/>
+      <c r="A14" s="21"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="27"/>
+      <c r="A15" s="21"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="27"/>
+      <c r="A16" s="21"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="27"/>
+      <c r="A17" s="21"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="27"/>
+      <c r="A18" s="21"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="27"/>
+      <c r="A19" s="21"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="27"/>
+      <c r="A20" s="21"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="27"/>
+      <c r="A21" s="21"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="27"/>
+      <c r="A22" s="21"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="27"/>
+      <c r="A23" s="21"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="27"/>
+      <c r="A24" s="21"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="27"/>
+      <c r="A25" s="21"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="27"/>
+      <c r="A26" s="21"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="27"/>
+      <c r="A27" s="21"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="27"/>
+      <c r="A28" s="21"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="27"/>
+      <c r="A29" s="21"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="27"/>
+      <c r="A30" s="21"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="27"/>
+      <c r="A31" s="21"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="27"/>
+      <c r="A32" s="21"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="27"/>
+      <c r="A33" s="21"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="27"/>
+      <c r="A34" s="21"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="27"/>
+      <c r="A35" s="21"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="27"/>
+      <c r="A36" s="21"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="27"/>
+      <c r="A37" s="21"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="27"/>
+      <c r="A38" s="21"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="27"/>
+      <c r="A39" s="21"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="27"/>
+      <c r="A40" s="21"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="27"/>
+      <c r="A41" s="21"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="27"/>
+      <c r="A42" s="21"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="27"/>
+      <c r="A43" s="21"/>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="27"/>
+      <c r="A44" s="21"/>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="27"/>
+      <c r="A45" s="21"/>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="27"/>
+      <c r="A46" s="21"/>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="27"/>
+      <c r="A47" s="21"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="27"/>
+      <c r="A48" s="21"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="27"/>
+      <c r="A49" s="21"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="27"/>
+      <c r="A50" s="21"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="27"/>
+      <c r="A51" s="21"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="27"/>
+      <c r="A52" s="21"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="27"/>
+      <c r="A53" s="21"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="27"/>
+      <c r="A54" s="21"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="27"/>
+      <c r="A55" s="21"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="27"/>
+      <c r="A56" s="21"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="27"/>
+      <c r="A57" s="21"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="27"/>
+      <c r="A58" s="21"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="27"/>
+      <c r="A59" s="21"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="27"/>
+      <c r="A60" s="21"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="27"/>
+      <c r="A61" s="21"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="27"/>
+      <c r="A62" s="21"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="27"/>
+      <c r="A63" s="21"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="27"/>
+      <c r="A64" s="21"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="27"/>
+      <c r="A65" s="21"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="27"/>
+      <c r="A66" s="21"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="27"/>
+      <c r="A67" s="21"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="27"/>
+      <c r="A68" s="21"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="27"/>
+      <c r="A69" s="21"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="27"/>
+      <c r="A70" s="21"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="27"/>
+      <c r="A71" s="21"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="27"/>
+      <c r="A72" s="21"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="27"/>
+      <c r="A73" s="21"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="27"/>
+      <c r="A74" s="21"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="27"/>
+      <c r="A75" s="21"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="27"/>
+      <c r="A76" s="21"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="27"/>
+      <c r="A77" s="21"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="27"/>
+      <c r="A78" s="21"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="27"/>
+      <c r="A79" s="21"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="27"/>
+      <c r="A80" s="21"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="27"/>
+      <c r="A81" s="21"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="27"/>
+      <c r="A82" s="21"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="27"/>
+      <c r="A83" s="21"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="27"/>
+      <c r="A84" s="21"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="27"/>
+      <c r="A85" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E1048576">

</xml_diff>